<commit_message>
Cache enum render value
</commit_message>
<xml_diff>
--- a/src/StaticSettingsTests/ValueRendererForEnums.Test.verified.xlsx
+++ b/src/StaticSettingsTests/ValueRendererForEnums.Test.verified.xlsx
@@ -25,10 +25,10 @@
     <t>Color</t>
   </si>
   <si>
-    <t>Build your dream</t>
+    <t>BUILDYOURDREAM</t>
   </si>
   <si>
-    <t>Antique white</t>
+    <t>ANTIQUEWHITE</t>
   </si>
 </sst>
 </file>
@@ -471,8 +471,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="13.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="19.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="15.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14" customHeight="1">

</xml_diff>

<commit_message>
Cache enum render value (#46)
</commit_message>
<xml_diff>
--- a/src/StaticSettingsTests/ValueRendererForEnums.Test.verified.xlsx
+++ b/src/StaticSettingsTests/ValueRendererForEnums.Test.verified.xlsx
@@ -25,10 +25,10 @@
     <t>Color</t>
   </si>
   <si>
-    <t>Build your dream</t>
+    <t>BUILDYOURDREAM</t>
   </si>
   <si>
-    <t>Antique white</t>
+    <t>ANTIQUEWHITE</t>
   </si>
 </sst>
 </file>
@@ -471,8 +471,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="13.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="19.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="15.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14" customHeight="1">

</xml_diff>